<commit_message>
change name of one flight in order to match folder naming
</commit_message>
<xml_diff>
--- a/data/Flight_Card_2017_AirData_in.xlsx
+++ b/data/Flight_Card_2017_AirData_in.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maximilianproll/OneDrive - Aalto-yliopisto/project_detect_bird_nests/data/Flights2017_Max/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maximilianproll/OneDrive - Aalto-yliopisto/project_detect_bird_nests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2369E1F0-760D-C24A-89D9-10CE9551916A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E149DCDB-4F29-9F45-BFFB-616718CEDB87}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8320" yWindow="460" windowWidth="15680" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -186,9 +186,6 @@
     <t>653-665</t>
   </si>
   <si>
-    <t>12_F1A_15</t>
-  </si>
-  <si>
     <t>294-314</t>
   </si>
   <si>
@@ -277,6 +274,9 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>12_F1a_15</t>
   </si>
 </sst>
 </file>
@@ -667,7 +667,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -739,13 +739,13 @@
         <v>16</v>
       </c>
       <c r="R1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="T1" s="11" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -1194,7 +1194,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
@@ -1225,7 +1225,7 @@
       </c>
       <c r="R12" s="1"/>
       <c r="S12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T12" s="1"/>
     </row>
@@ -1237,7 +1237,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="1">
         <v>2</v>
@@ -1268,10 +1268,10 @@
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T13" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="T13" s="10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
@@ -1282,7 +1282,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="R14" s="1"/>
       <c r="S14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T14" s="1"/>
     </row>
@@ -1325,7 +1325,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1">
         <v>5</v>
@@ -1355,13 +1355,13 @@
         <v>19</v>
       </c>
       <c r="R15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="S15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="S15" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="T15" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
@@ -1372,7 +1372,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="R16" s="1"/>
       <c r="S16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T16" s="1"/>
     </row>
@@ -1415,7 +1415,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -1447,7 +1447,7 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
@@ -1458,7 +1458,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1">
         <v>4</v>
@@ -1488,10 +1488,10 @@
         <v>19</v>
       </c>
       <c r="R18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S18" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="T18" s="1"/>
     </row>
@@ -1503,7 +1503,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" s="1">
         <v>2</v>
@@ -1534,10 +1534,10 @@
       </c>
       <c r="R19" s="1"/>
       <c r="S19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T19" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="T19" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
@@ -1548,7 +1548,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -1572,14 +1572,14 @@
         <v>86</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="R20" s="1"/>
       <c r="S20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T20" s="1"/>
     </row>
@@ -1591,7 +1591,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -1621,13 +1621,13 @@
         <v>19</v>
       </c>
       <c r="R21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S21" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="S21" s="1" t="s">
+      <c r="T21" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>